<commit_message>
Read description about 200+ files being committed
I organized my three sets of test cases (class times, prerequisites,
courses to schedule) into No Errors, One Error, and Many Errors to
simplify the printing and organizing we'll be doing later.  So Github is
counting all the tests I removed from their original location as well as
the files that were put into a new directory (from when I moved test
files).

Also, I editted the class times index just a little.  I had apparently
marked a file incorrect that was actually incorrect, as pointed out by
Alla.
</commit_message>
<xml_diff>
--- a/TestFiles/classtimes/classtimesindex.xlsx
+++ b/TestFiles/classtimes/classtimesindex.xlsx
@@ -39,9 +39,6 @@
     <t>Input is not accepted.  Potential keystroke error.  Should be W instead of Q.</t>
   </si>
   <si>
-    <t>Input is not accepted.  Expected slash in line 4.</t>
-  </si>
-  <si>
     <t>Input is not accepted.  Day of week is spelled instead of abbreviated in line 17.</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t xml:space="preserve"> classt030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input is accepted.  </t>
   </si>
 </sst>
 </file>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,23 +572,23 @@
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -612,135 +612,135 @@
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>6</v>
@@ -748,31 +748,31 @@
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
@@ -780,34 +780,34 @@
     </row>
     <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>